<commit_message>
Cambios finales en el presupuesto
</commit_message>
<xml_diff>
--- a/ENTREGA/HITO0/Plantilla_Presupuesto_ABP_2016-17.xlsx
+++ b/ENTREGA/HITO0/Plantilla_Presupuesto_ABP_2016-17.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1458" uniqueCount="586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="586">
   <si>
     <t>Apellidos</t>
   </si>
@@ -4887,20 +4887,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="46" xfId="145" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="145" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="44" xfId="145" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="45" xfId="145" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="145" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="46" xfId="145" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="13" borderId="1" xfId="145" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4913,6 +4904,15 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="14" borderId="1" xfId="145" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="44" xfId="145" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="45" xfId="145" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="145" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -12320,32 +12320,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="23.25">
-      <c r="A1" s="265" t="s">
+      <c r="A1" s="270" t="s">
         <v>210</v>
       </c>
-      <c r="B1" s="265"/>
-      <c r="C1" s="265"/>
-      <c r="D1" s="265"/>
-      <c r="E1" s="265"/>
-      <c r="F1" s="265"/>
-      <c r="G1" s="265"/>
-      <c r="H1" s="265"/>
-      <c r="I1" s="265"/>
-      <c r="J1" s="265"/>
+      <c r="B1" s="270"/>
+      <c r="C1" s="270"/>
+      <c r="D1" s="270"/>
+      <c r="E1" s="270"/>
+      <c r="F1" s="270"/>
+      <c r="G1" s="270"/>
+      <c r="H1" s="270"/>
+      <c r="I1" s="270"/>
+      <c r="J1" s="270"/>
     </row>
     <row r="2" spans="1:10" ht="96" customHeight="1" thickBot="1">
-      <c r="A2" s="266" t="s">
+      <c r="A2" s="271" t="s">
         <v>211</v>
       </c>
-      <c r="B2" s="266"/>
-      <c r="C2" s="266"/>
-      <c r="D2" s="266"/>
-      <c r="E2" s="266"/>
-      <c r="F2" s="266"/>
-      <c r="G2" s="266"/>
-      <c r="H2" s="266"/>
-      <c r="I2" s="266"/>
-      <c r="J2" s="266"/>
+      <c r="B2" s="271"/>
+      <c r="C2" s="271"/>
+      <c r="D2" s="271"/>
+      <c r="E2" s="271"/>
+      <c r="F2" s="271"/>
+      <c r="G2" s="271"/>
+      <c r="H2" s="271"/>
+      <c r="I2" s="271"/>
+      <c r="J2" s="271"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="67"/>
@@ -12360,20 +12360,20 @@
       <c r="J3" s="67"/>
     </row>
     <row r="4" spans="1:10" ht="20.85" customHeight="1">
-      <c r="A4" s="267" t="s">
+      <c r="A4" s="272" t="s">
         <v>212</v>
       </c>
-      <c r="B4" s="267"/>
+      <c r="B4" s="272"/>
       <c r="C4" s="67"/>
-      <c r="D4" s="267" t="s">
+      <c r="D4" s="272" t="s">
         <v>213</v>
       </c>
-      <c r="E4" s="267"/>
-      <c r="F4" s="267"/>
-      <c r="G4" s="267"/>
-      <c r="H4" s="267"/>
-      <c r="I4" s="267"/>
-      <c r="J4" s="267"/>
+      <c r="E4" s="272"/>
+      <c r="F4" s="272"/>
+      <c r="G4" s="272"/>
+      <c r="H4" s="272"/>
+      <c r="I4" s="272"/>
+      <c r="J4" s="272"/>
     </row>
     <row r="5" spans="1:10" ht="15.75">
       <c r="A5" s="68" t="s">
@@ -12383,14 +12383,14 @@
         <v>215</v>
       </c>
       <c r="C5" s="67"/>
-      <c r="D5" s="264" t="s">
+      <c r="D5" s="265" t="s">
         <v>216</v>
       </c>
-      <c r="E5" s="264"/>
-      <c r="F5" s="264"/>
-      <c r="G5" s="264"/>
-      <c r="H5" s="264"/>
-      <c r="I5" s="264"/>
+      <c r="E5" s="265"/>
+      <c r="F5" s="265"/>
+      <c r="G5" s="265"/>
+      <c r="H5" s="265"/>
+      <c r="I5" s="265"/>
       <c r="J5" s="70">
         <f>'Principal - ABP'!G19</f>
         <v>6</v>
@@ -12404,14 +12404,14 @@
         <v>10</v>
       </c>
       <c r="C6" s="67"/>
-      <c r="D6" s="264" t="s">
+      <c r="D6" s="265" t="s">
         <v>218</v>
       </c>
-      <c r="E6" s="264"/>
-      <c r="F6" s="264"/>
-      <c r="G6" s="264"/>
-      <c r="H6" s="264"/>
-      <c r="I6" s="264"/>
+      <c r="E6" s="265"/>
+      <c r="F6" s="265"/>
+      <c r="G6" s="265"/>
+      <c r="H6" s="265"/>
+      <c r="I6" s="265"/>
       <c r="J6" s="72">
         <f>J5*B7</f>
         <v>660</v>
@@ -12425,14 +12425,14 @@
         <v>110</v>
       </c>
       <c r="C7" s="67"/>
-      <c r="D7" s="264" t="s">
+      <c r="D7" s="265" t="s">
         <v>220</v>
       </c>
-      <c r="E7" s="264"/>
-      <c r="F7" s="264"/>
-      <c r="G7" s="264"/>
-      <c r="H7" s="264"/>
-      <c r="I7" s="264"/>
+      <c r="E7" s="265"/>
+      <c r="F7" s="265"/>
+      <c r="G7" s="265"/>
+      <c r="H7" s="265"/>
+      <c r="I7" s="265"/>
       <c r="J7" s="73">
         <f>I13</f>
         <v>694</v>
@@ -12446,14 +12446,14 @@
         <v>30</v>
       </c>
       <c r="C8" s="67"/>
-      <c r="D8" s="264" t="s">
+      <c r="D8" s="265" t="s">
         <v>222</v>
       </c>
-      <c r="E8" s="264"/>
-      <c r="F8" s="264"/>
-      <c r="G8" s="264"/>
-      <c r="H8" s="264"/>
-      <c r="I8" s="264"/>
+      <c r="E8" s="265"/>
+      <c r="F8" s="265"/>
+      <c r="G8" s="265"/>
+      <c r="H8" s="265"/>
+      <c r="I8" s="265"/>
       <c r="J8" s="74">
         <f>ABS(J6-J7)/J6</f>
         <v>5.1515151515151514E-2</v>
@@ -12468,14 +12468,14 @@
         <v>150</v>
       </c>
       <c r="C9" s="67"/>
-      <c r="D9" s="269" t="s">
+      <c r="D9" s="266" t="s">
         <v>223</v>
       </c>
-      <c r="E9" s="269"/>
-      <c r="F9" s="269"/>
-      <c r="G9" s="269"/>
-      <c r="H9" s="269"/>
-      <c r="I9" s="269"/>
+      <c r="E9" s="266"/>
+      <c r="F9" s="266"/>
+      <c r="G9" s="266"/>
+      <c r="H9" s="266"/>
+      <c r="I9" s="266"/>
       <c r="J9" s="77">
         <f>J13</f>
         <v>63.090909090909079</v>
@@ -12494,37 +12494,37 @@
       <c r="J10" s="67"/>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1">
-      <c r="A11" s="270" t="s">
+      <c r="A11" s="267" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="270" t="s">
+      <c r="B11" s="267" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="270" t="s">
+      <c r="C11" s="267" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="271" t="s">
+      <c r="D11" s="268" t="s">
         <v>224</v>
       </c>
-      <c r="E11" s="272" t="s">
+      <c r="E11" s="269" t="s">
         <v>225</v>
       </c>
-      <c r="F11" s="271" t="s">
+      <c r="F11" s="268" t="s">
         <v>226</v>
       </c>
-      <c r="G11" s="271"/>
-      <c r="H11" s="271"/>
-      <c r="I11" s="272" t="s">
+      <c r="G11" s="268"/>
+      <c r="H11" s="268"/>
+      <c r="I11" s="269" t="s">
         <v>227</v>
       </c>
-      <c r="J11" s="272"/>
+      <c r="J11" s="269"/>
     </row>
     <row r="12" spans="1:10" ht="14.25">
-      <c r="A12" s="270"/>
-      <c r="B12" s="270"/>
-      <c r="C12" s="270"/>
-      <c r="D12" s="271"/>
-      <c r="E12" s="271"/>
+      <c r="A12" s="267"/>
+      <c r="B12" s="267"/>
+      <c r="C12" s="267"/>
+      <c r="D12" s="268"/>
+      <c r="E12" s="268"/>
       <c r="F12" s="78" t="s">
         <v>228</v>
       </c>
@@ -12542,14 +12542,14 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="18.75">
-      <c r="A13" s="268"/>
-      <c r="B13" s="268"/>
-      <c r="C13" s="268"/>
-      <c r="D13" s="268"/>
-      <c r="E13" s="268"/>
-      <c r="F13" s="268"/>
-      <c r="G13" s="268"/>
-      <c r="H13" s="268"/>
+      <c r="A13" s="264"/>
+      <c r="B13" s="264"/>
+      <c r="C13" s="264"/>
+      <c r="D13" s="264"/>
+      <c r="E13" s="264"/>
+      <c r="F13" s="264"/>
+      <c r="G13" s="264"/>
+      <c r="H13" s="264"/>
       <c r="I13" s="80">
         <f>SUM(I14:I49)</f>
         <v>694</v>
@@ -13711,6 +13711,12 @@
   </sheetData>
   <sheetProtection password="C894" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="17">
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:J4"/>
+    <mergeCell ref="D5:I5"/>
     <mergeCell ref="A13:H13"/>
     <mergeCell ref="D7:I7"/>
     <mergeCell ref="D8:I8"/>
@@ -13722,12 +13728,6 @@
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="I11:J11"/>
-    <mergeCell ref="D6:I6"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:J4"/>
-    <mergeCell ref="D5:I5"/>
   </mergeCells>
   <conditionalFormatting sqref="J8">
     <cfRule type="cellIs" dxfId="27" priority="1" operator="greaterThan">
@@ -13755,8 +13755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="12.75"/>
@@ -13768,32 +13768,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="23.25">
-      <c r="A1" s="265" t="s">
+      <c r="A1" s="270" t="s">
         <v>315</v>
       </c>
-      <c r="B1" s="265"/>
-      <c r="C1" s="265"/>
-      <c r="D1" s="265"/>
-      <c r="E1" s="265"/>
-      <c r="F1" s="265"/>
-      <c r="G1" s="265"/>
-      <c r="H1" s="265"/>
-      <c r="I1" s="265"/>
-      <c r="J1" s="265"/>
+      <c r="B1" s="270"/>
+      <c r="C1" s="270"/>
+      <c r="D1" s="270"/>
+      <c r="E1" s="270"/>
+      <c r="F1" s="270"/>
+      <c r="G1" s="270"/>
+      <c r="H1" s="270"/>
+      <c r="I1" s="270"/>
+      <c r="J1" s="270"/>
     </row>
     <row r="2" spans="1:10" ht="96" customHeight="1" thickBot="1">
-      <c r="A2" s="266" t="s">
+      <c r="A2" s="271" t="s">
         <v>211</v>
       </c>
-      <c r="B2" s="266"/>
-      <c r="C2" s="266"/>
-      <c r="D2" s="266"/>
-      <c r="E2" s="266"/>
-      <c r="F2" s="266"/>
-      <c r="G2" s="266"/>
-      <c r="H2" s="266"/>
-      <c r="I2" s="266"/>
-      <c r="J2" s="266"/>
+      <c r="B2" s="271"/>
+      <c r="C2" s="271"/>
+      <c r="D2" s="271"/>
+      <c r="E2" s="271"/>
+      <c r="F2" s="271"/>
+      <c r="G2" s="271"/>
+      <c r="H2" s="271"/>
+      <c r="I2" s="271"/>
+      <c r="J2" s="271"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="67"/>
@@ -13808,20 +13808,20 @@
       <c r="J3" s="67"/>
     </row>
     <row r="4" spans="1:10" ht="20.85" customHeight="1">
-      <c r="A4" s="267" t="s">
+      <c r="A4" s="272" t="s">
         <v>212</v>
       </c>
-      <c r="B4" s="267"/>
+      <c r="B4" s="272"/>
       <c r="C4" s="67"/>
-      <c r="D4" s="267" t="s">
+      <c r="D4" s="272" t="s">
         <v>213</v>
       </c>
-      <c r="E4" s="267"/>
-      <c r="F4" s="267"/>
-      <c r="G4" s="267"/>
-      <c r="H4" s="267"/>
-      <c r="I4" s="267"/>
-      <c r="J4" s="267"/>
+      <c r="E4" s="272"/>
+      <c r="F4" s="272"/>
+      <c r="G4" s="272"/>
+      <c r="H4" s="272"/>
+      <c r="I4" s="272"/>
+      <c r="J4" s="272"/>
     </row>
     <row r="5" spans="1:10" ht="15.75">
       <c r="A5" s="68" t="s">
@@ -13831,14 +13831,14 @@
         <v>215</v>
       </c>
       <c r="C5" s="67"/>
-      <c r="D5" s="264" t="s">
+      <c r="D5" s="265" t="s">
         <v>216</v>
       </c>
-      <c r="E5" s="264"/>
-      <c r="F5" s="264"/>
-      <c r="G5" s="264"/>
-      <c r="H5" s="264"/>
-      <c r="I5" s="264"/>
+      <c r="E5" s="265"/>
+      <c r="F5" s="265"/>
+      <c r="G5" s="265"/>
+      <c r="H5" s="265"/>
+      <c r="I5" s="265"/>
       <c r="J5" s="70">
         <f>'Principal - ABP'!G19</f>
         <v>6</v>
@@ -13852,14 +13852,14 @@
         <v>10</v>
       </c>
       <c r="C6" s="67"/>
-      <c r="D6" s="264" t="s">
+      <c r="D6" s="265" t="s">
         <v>218</v>
       </c>
-      <c r="E6" s="264"/>
-      <c r="F6" s="264"/>
-      <c r="G6" s="264"/>
-      <c r="H6" s="264"/>
-      <c r="I6" s="264"/>
+      <c r="E6" s="265"/>
+      <c r="F6" s="265"/>
+      <c r="G6" s="265"/>
+      <c r="H6" s="265"/>
+      <c r="I6" s="265"/>
       <c r="J6" s="72">
         <f>J5*B7</f>
         <v>660</v>
@@ -13873,17 +13873,17 @@
         <v>110</v>
       </c>
       <c r="C7" s="67"/>
-      <c r="D7" s="264" t="s">
+      <c r="D7" s="265" t="s">
         <v>220</v>
       </c>
-      <c r="E7" s="264"/>
-      <c r="F7" s="264"/>
-      <c r="G7" s="264"/>
-      <c r="H7" s="264"/>
-      <c r="I7" s="264"/>
+      <c r="E7" s="265"/>
+      <c r="F7" s="265"/>
+      <c r="G7" s="265"/>
+      <c r="H7" s="265"/>
+      <c r="I7" s="265"/>
       <c r="J7" s="73">
         <f>I13</f>
-        <v>660</v>
+        <v>665</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="20.25" customHeight="1">
@@ -13894,17 +13894,17 @@
         <v>30</v>
       </c>
       <c r="C8" s="67"/>
-      <c r="D8" s="264" t="s">
+      <c r="D8" s="265" t="s">
         <v>222</v>
       </c>
-      <c r="E8" s="264"/>
-      <c r="F8" s="264"/>
-      <c r="G8" s="264"/>
-      <c r="H8" s="264"/>
-      <c r="I8" s="264"/>
+      <c r="E8" s="265"/>
+      <c r="F8" s="265"/>
+      <c r="G8" s="265"/>
+      <c r="H8" s="265"/>
+      <c r="I8" s="265"/>
       <c r="J8" s="74">
         <f>ABS(J6-J7)/J6</f>
-        <v>0</v>
+        <v>7.575757575757576E-3</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="18.75">
@@ -13916,17 +13916,17 @@
         <v>150</v>
       </c>
       <c r="C9" s="67"/>
-      <c r="D9" s="269" t="s">
+      <c r="D9" s="266" t="s">
         <v>223</v>
       </c>
-      <c r="E9" s="269"/>
-      <c r="F9" s="269"/>
-      <c r="G9" s="269"/>
-      <c r="H9" s="269"/>
-      <c r="I9" s="269"/>
+      <c r="E9" s="266"/>
+      <c r="F9" s="266"/>
+      <c r="G9" s="266"/>
+      <c r="H9" s="266"/>
+      <c r="I9" s="266"/>
       <c r="J9" s="77">
         <f>J13</f>
-        <v>60.000000000000007</v>
+        <v>60.454545454545453</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -13942,37 +13942,37 @@
       <c r="J10" s="67"/>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1">
-      <c r="A11" s="270" t="s">
+      <c r="A11" s="267" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="270" t="s">
+      <c r="B11" s="267" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="270" t="s">
+      <c r="C11" s="267" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="271" t="s">
+      <c r="D11" s="268" t="s">
         <v>224</v>
       </c>
-      <c r="E11" s="272" t="s">
+      <c r="E11" s="269" t="s">
         <v>225</v>
       </c>
-      <c r="F11" s="271" t="s">
+      <c r="F11" s="268" t="s">
         <v>226</v>
       </c>
-      <c r="G11" s="271"/>
-      <c r="H11" s="271"/>
-      <c r="I11" s="272" t="s">
+      <c r="G11" s="268"/>
+      <c r="H11" s="268"/>
+      <c r="I11" s="269" t="s">
         <v>227</v>
       </c>
-      <c r="J11" s="272"/>
+      <c r="J11" s="269"/>
     </row>
     <row r="12" spans="1:10" ht="14.25">
-      <c r="A12" s="270"/>
-      <c r="B12" s="270"/>
-      <c r="C12" s="270"/>
-      <c r="D12" s="271"/>
-      <c r="E12" s="271"/>
+      <c r="A12" s="267"/>
+      <c r="B12" s="267"/>
+      <c r="C12" s="267"/>
+      <c r="D12" s="268"/>
+      <c r="E12" s="268"/>
       <c r="F12" s="78" t="s">
         <v>228</v>
       </c>
@@ -13990,21 +13990,21 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="18.75">
-      <c r="A13" s="268"/>
-      <c r="B13" s="268"/>
-      <c r="C13" s="268"/>
-      <c r="D13" s="268"/>
-      <c r="E13" s="268"/>
-      <c r="F13" s="268"/>
-      <c r="G13" s="268"/>
-      <c r="H13" s="268"/>
+      <c r="A13" s="264"/>
+      <c r="B13" s="264"/>
+      <c r="C13" s="264"/>
+      <c r="D13" s="264"/>
+      <c r="E13" s="264"/>
+      <c r="F13" s="264"/>
+      <c r="G13" s="264"/>
+      <c r="H13" s="264"/>
       <c r="I13" s="80">
         <f>SUM(I14:I48)</f>
-        <v>660</v>
+        <v>665</v>
       </c>
       <c r="J13" s="80">
         <f>SUM(J14:J48)</f>
-        <v>60.000000000000007</v>
+        <v>60.454545454545453</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="31.5">
@@ -14020,8 +14020,8 @@
       <c r="D14" s="81" t="s">
         <v>319</v>
       </c>
-      <c r="E14" s="84">
-        <v>1</v>
+      <c r="E14" s="84" t="s">
+        <v>584</v>
       </c>
       <c r="F14" s="85">
         <v>5</v>
@@ -14034,11 +14034,11 @@
         <v>55</v>
       </c>
       <c r="I14" s="87">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="J14" s="88">
         <f>I14/$J$6*10*$J$5</f>
-        <v>5.454545454545455</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="31.5">
@@ -14054,8 +14054,8 @@
       <c r="D15" s="81" t="s">
         <v>319</v>
       </c>
-      <c r="E15" s="84" t="s">
-        <v>584</v>
+      <c r="E15" s="84">
+        <v>1</v>
       </c>
       <c r="F15" s="85">
         <v>10</v>
@@ -14067,10 +14067,12 @@
         <f t="shared" si="0"/>
         <v>85</v>
       </c>
-      <c r="I15" s="87"/>
+      <c r="I15" s="87">
+        <v>85</v>
+      </c>
       <c r="J15" s="88">
         <f t="shared" ref="J15:J48" si="1">I15/$J$6*10*$J$5</f>
-        <v>0</v>
+        <v>7.7272727272727266</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75">
@@ -14912,8 +14914,8 @@
       <c r="D41" s="81" t="s">
         <v>374</v>
       </c>
-      <c r="E41" s="84">
-        <v>2</v>
+      <c r="E41" s="84" t="s">
+        <v>584</v>
       </c>
       <c r="F41" s="85">
         <v>2</v>
@@ -14926,11 +14928,11 @@
         <v>17</v>
       </c>
       <c r="I41" s="87">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="J41" s="88">
         <f t="shared" si="1"/>
-        <v>1.8181818181818183</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="31.5">
@@ -15156,12 +15158,6 @@
   </sheetData>
   <sheetProtection password="C894" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="17">
-    <mergeCell ref="D6:I6"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:J4"/>
-    <mergeCell ref="D5:I5"/>
     <mergeCell ref="A13:H13"/>
     <mergeCell ref="D7:I7"/>
     <mergeCell ref="D8:I8"/>
@@ -15173,6 +15169,12 @@
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="I11:J11"/>
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:J4"/>
+    <mergeCell ref="D5:I5"/>
   </mergeCells>
   <conditionalFormatting sqref="J8">
     <cfRule type="cellIs" dxfId="25" priority="1" operator="greaterThan">

</xml_diff>